<commit_message>
Minor fixes on template
Minor text fixes
</commit_message>
<xml_diff>
--- a/TestData/Manually extracted minutiae/Normal/Template_Ale1439794734-Hamster-0-1.xlsx
+++ b/TestData/Manually extracted minutiae/Normal/Template_Ale1439794734-Hamster-0-1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag720\Desktop\Tagged minutiae\libAFIS\TestData\Perfect minutiae\Normal fingers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.carrera\Documents\GitHub\libAFIS\TestData\Manually extracted minutiae\Normal\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Collected Minutiae" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>X</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Minutiae data</t>
   </si>
   <si>
-    <t>Finger Header</t>
-  </si>
-  <si>
     <t>Finger header</t>
   </si>
   <si>
@@ -88,12 +85,6 @@
     <t>80</t>
   </si>
   <si>
-    <t>4087000B6600</t>
-  </si>
-  <si>
-    <t>464D52002032300000000144000000C0010C00C800C8010000006301</t>
-  </si>
-  <si>
     <t>464D520020323000000000</t>
   </si>
   <si>
@@ -113,6 +104,18 @@
   </si>
   <si>
     <t>0000</t>
+  </si>
+  <si>
+    <t>Bifurcation</t>
+  </si>
+  <si>
+    <t>Ending</t>
+  </si>
+  <si>
+    <t>Finger Header Top</t>
+  </si>
+  <si>
+    <t>Finger Header Bottom</t>
   </si>
 </sst>
 </file>
@@ -162,7 +165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -180,9 +183,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -195,10 +196,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +479,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:V5"/>
     </sheetView>
   </sheetViews>
@@ -520,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -540,10 +537,10 @@
         <v>6</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -551,7 +548,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>135.91800000000001</v>
@@ -605,7 +602,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <v>181.63300000000001</v>
@@ -653,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>113.06100000000001</v>
@@ -700,7 +697,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>118.776</v>
@@ -747,7 +744,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>160</v>
@@ -788,7 +785,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <v>143</v>
@@ -829,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>90</v>
@@ -870,7 +867,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <v>65</v>
@@ -906,7 +903,7 @@
         <v>80410065FC00</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:22" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -914,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>125</v>
@@ -959,7 +956,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11">
         <v>53.061</v>
@@ -1000,7 +997,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12">
         <v>170.20400000000001</v>
@@ -1041,7 +1038,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>107.34699999999999</v>
@@ -1082,7 +1079,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>92.245000000000005</v>
@@ -1123,7 +1120,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15">
         <v>69.796000000000006</v>
@@ -1164,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16">
         <v>44.082000000000001</v>
@@ -1205,7 +1202,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>156.73500000000001</v>
@@ -1246,7 +1243,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18">
         <v>54.286000000000001</v>
@@ -1287,7 +1284,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19">
         <v>70.611999999999995</v>
@@ -1328,7 +1325,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20">
         <v>45.305999999999997</v>
@@ -1369,7 +1366,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21">
         <v>102.041</v>
@@ -1410,7 +1407,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C22">
         <v>175.102</v>
@@ -1451,7 +1448,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23">
         <v>150.61199999999999</v>
@@ -1492,7 +1489,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <v>85.305999999999997</v>
@@ -1533,7 +1530,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25">
         <v>162.44900000000001</v>
@@ -1574,7 +1571,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26">
         <v>81.224000000000004</v>
@@ -1615,7 +1612,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27">
         <v>55.51</v>
@@ -1656,7 +1653,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>72.245000000000005</v>
@@ -1697,7 +1694,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29">
         <v>122.857</v>
@@ -1738,7 +1735,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30">
         <v>106.122</v>
@@ -1779,7 +1776,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C31">
         <v>167.34700000000001</v>
@@ -1820,7 +1817,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>93.468999999999994</v>
@@ -1861,7 +1858,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C33">
         <v>153.06100000000001</v>
@@ -1920,7 +1917,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1937,14 +1934,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1970,24 +1968,28 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -2054,21 +2056,21 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="13" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="9"/>
+      <c r="B12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="13"/>
       <c r="D12" t="str">
         <f>DEC2HEX(SUM(27,(6*D15),3))</f>
         <v>DE</v>
@@ -2078,10 +2080,12 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="13"/>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -2089,7 +2093,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="1" t="str">
@@ -2099,12 +2103,12 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="1"/>
+      <c r="B15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="12"/>
       <c r="D15" s="1">
         <f>COUNT('Collected Minutiae'!A2:A1000)</f>
         <v>32</v>
@@ -2114,34 +2118,21 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="str">
-        <f>CONCATENATE(C21,C22,0)</f>
-        <v>464D52002032300000000144000000C0010C00C800C80100000063014087000B66000</v>
+        <v>24</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>